<commit_message>
added scraping data for li17
</commit_message>
<xml_diff>
--- a/data/egret_JS/egret_JS.xlsx
+++ b/data/egret_JS/egret_JS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\julie\EGRET\egret\data\egret_JS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4710AFAB-0AA0-4270-88FC-048FB5B2C3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C931EEA-0ABD-450E-A33F-20664DDD0ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="-17400" windowWidth="30960" windowHeight="16920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_general" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14376" uniqueCount="2690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15037" uniqueCount="2711">
   <si>
     <t>datasetID</t>
   </si>
@@ -8122,6 +8122,69 @@
   </si>
   <si>
     <t>In Chinese</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R </t>
+  </si>
+  <si>
+    <t>112.26667 E</t>
+  </si>
+  <si>
+    <t>31.0333 N</t>
+  </si>
+  <si>
+    <t>Wangusi Village, Guizhou Town, Zigui County, Yichang City, Hubei Province, China</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>cold sand</t>
+  </si>
+  <si>
+    <t>50 - 60</t>
+  </si>
+  <si>
+    <t>cold dry</t>
+  </si>
+  <si>
+    <t>room temp sand</t>
+  </si>
+  <si>
+    <t>avg 17</t>
+  </si>
+  <si>
+    <t>room temp dry</t>
+  </si>
+  <si>
+    <t>avg 18</t>
+  </si>
+  <si>
+    <t>cold sand storage</t>
+  </si>
+  <si>
+    <t>cold dry storage</t>
+  </si>
+  <si>
+    <t>room sand storage</t>
+  </si>
+  <si>
+    <t>room dry storage</t>
+  </si>
+  <si>
+    <t>cold start</t>
+  </si>
+  <si>
+    <t>25/15</t>
+  </si>
+  <si>
+    <t>16/8</t>
+  </si>
+  <si>
+    <t>no storage</t>
   </si>
 </sst>
 </file>
@@ -8277,7 +8340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8481,6 +8544,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -8670,7 +8739,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8691,6 +8760,9 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -9082,8 +9154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -9653,8 +9725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B357" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A394" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C474" sqref="C474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -18849,7 +18921,13 @@
         <v>1202</v>
       </c>
       <c r="K191" t="s">
-        <v>151</v>
+        <v>2691</v>
+      </c>
+      <c r="L191" t="s">
+        <v>2689</v>
+      </c>
+      <c r="M191" t="s">
+        <v>2690</v>
       </c>
       <c r="P191" t="s">
         <v>755</v>
@@ -32145,10 +32223,13 @@
         <v>2571</v>
       </c>
       <c r="K485" t="s">
-        <v>151</v>
+        <v>297</v>
       </c>
       <c r="L485" t="s">
         <v>2689</v>
+      </c>
+      <c r="M485" t="s">
+        <v>2690</v>
       </c>
       <c r="R485" t="s">
         <v>239</v>
@@ -32305,11 +32386,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AS282"/>
+  <dimension ref="A1:AS296"/>
   <sheetViews>
-    <sheetView zoomScale="76" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR265" sqref="AR265:AR282"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AP303" sqref="AP303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -67371,10 +67452,10 @@
       <c r="AF262" t="s">
         <v>40</v>
       </c>
-      <c r="AG262" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH262" t="s">
+      <c r="AG262" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH262" s="15" t="s">
         <v>39</v>
       </c>
       <c r="AI262" t="s">
@@ -67505,10 +67586,10 @@
       <c r="AF263" t="s">
         <v>40</v>
       </c>
-      <c r="AG263" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH263" t="s">
+      <c r="AG263" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH263" s="15" t="s">
         <v>39</v>
       </c>
       <c r="AI263" t="s">
@@ -67633,17 +67714,17 @@
       <c r="AD264" t="s">
         <v>40</v>
       </c>
-      <c r="AE264" t="s">
-        <v>40</v>
+      <c r="AE264" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF264" t="s">
         <v>40</v>
       </c>
-      <c r="AG264" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH264" t="s">
-        <v>40</v>
+      <c r="AG264" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH264" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI264" t="s">
         <v>40</v>
@@ -67767,17 +67848,17 @@
       <c r="AD265" t="s">
         <v>40</v>
       </c>
-      <c r="AE265" t="s">
-        <v>40</v>
+      <c r="AE265" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF265" t="s">
         <v>40</v>
       </c>
-      <c r="AG265" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH265" t="s">
-        <v>40</v>
+      <c r="AG265" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH265" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI265" t="s">
         <v>40</v>
@@ -67901,17 +67982,17 @@
       <c r="AD266" t="s">
         <v>40</v>
       </c>
-      <c r="AE266" t="s">
-        <v>40</v>
+      <c r="AE266" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF266" t="s">
         <v>40</v>
       </c>
-      <c r="AG266" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH266" t="s">
-        <v>40</v>
+      <c r="AG266" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH266" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI266" t="s">
         <v>40</v>
@@ -68035,17 +68116,17 @@
       <c r="AD267" t="s">
         <v>40</v>
       </c>
-      <c r="AE267" t="s">
-        <v>40</v>
+      <c r="AE267" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF267" t="s">
         <v>40</v>
       </c>
-      <c r="AG267" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH267" t="s">
-        <v>40</v>
+      <c r="AG267" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH267" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI267" t="s">
         <v>40</v>
@@ -68169,17 +68250,17 @@
       <c r="AD268" t="s">
         <v>40</v>
       </c>
-      <c r="AE268" t="s">
-        <v>40</v>
+      <c r="AE268" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF268" t="s">
         <v>40</v>
       </c>
-      <c r="AG268" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH268" t="s">
-        <v>40</v>
+      <c r="AG268" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH268" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI268" t="s">
         <v>40</v>
@@ -68303,17 +68384,17 @@
       <c r="AD269" t="s">
         <v>40</v>
       </c>
-      <c r="AE269" t="s">
-        <v>40</v>
+      <c r="AE269" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF269" t="s">
         <v>40</v>
       </c>
-      <c r="AG269" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH269" t="s">
-        <v>40</v>
+      <c r="AG269" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH269" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI269" t="s">
         <v>40</v>
@@ -68437,17 +68518,17 @@
       <c r="AD270" t="s">
         <v>40</v>
       </c>
-      <c r="AE270" t="s">
-        <v>40</v>
+      <c r="AE270" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF270" t="s">
         <v>40</v>
       </c>
-      <c r="AG270" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH270" t="s">
-        <v>40</v>
+      <c r="AG270" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH270" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI270" t="s">
         <v>40</v>
@@ -68571,17 +68652,17 @@
       <c r="AD271" t="s">
         <v>40</v>
       </c>
-      <c r="AE271" t="s">
-        <v>40</v>
+      <c r="AE271" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF271" t="s">
         <v>40</v>
       </c>
-      <c r="AG271" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH271" t="s">
-        <v>40</v>
+      <c r="AG271" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH271" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI271" t="s">
         <v>40</v>
@@ -68705,17 +68786,17 @@
       <c r="AD272" t="s">
         <v>40</v>
       </c>
-      <c r="AE272" t="s">
-        <v>40</v>
+      <c r="AE272" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF272" t="s">
         <v>40</v>
       </c>
-      <c r="AG272" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH272" t="s">
-        <v>40</v>
+      <c r="AG272" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH272" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI272" t="s">
         <v>40</v>
@@ -68748,7 +68829,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="273" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="273" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A273" t="s">
         <v>2581</v>
       </c>
@@ -68839,17 +68920,17 @@
       <c r="AD273" t="s">
         <v>40</v>
       </c>
-      <c r="AE273" t="s">
-        <v>40</v>
+      <c r="AE273" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF273" t="s">
         <v>40</v>
       </c>
-      <c r="AG273" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH273" t="s">
-        <v>40</v>
+      <c r="AG273" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH273" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI273" t="s">
         <v>40</v>
@@ -68882,7 +68963,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="274" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="274" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A274" t="s">
         <v>2581</v>
       </c>
@@ -68973,17 +69054,17 @@
       <c r="AD274" t="s">
         <v>40</v>
       </c>
-      <c r="AE274" t="s">
-        <v>40</v>
+      <c r="AE274" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF274" t="s">
         <v>40</v>
       </c>
-      <c r="AG274" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH274" t="s">
-        <v>40</v>
+      <c r="AG274" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH274" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI274" t="s">
         <v>40</v>
@@ -69016,7 +69097,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="275" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="275" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A275" t="s">
         <v>2581</v>
       </c>
@@ -69107,17 +69188,17 @@
       <c r="AD275" t="s">
         <v>40</v>
       </c>
-      <c r="AE275" t="s">
-        <v>40</v>
+      <c r="AE275" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF275" t="s">
         <v>40</v>
       </c>
-      <c r="AG275" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH275" t="s">
-        <v>40</v>
+      <c r="AG275" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH275" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI275" t="s">
         <v>40</v>
@@ -69150,7 +69231,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="276" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="276" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A276" t="s">
         <v>2581</v>
       </c>
@@ -69241,17 +69322,17 @@
       <c r="AD276" t="s">
         <v>40</v>
       </c>
-      <c r="AE276" t="s">
-        <v>40</v>
+      <c r="AE276" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF276" t="s">
         <v>40</v>
       </c>
-      <c r="AG276" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH276" t="s">
-        <v>40</v>
+      <c r="AG276" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH276" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI276" t="s">
         <v>40</v>
@@ -69284,7 +69365,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="277" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="277" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A277" t="s">
         <v>2581</v>
       </c>
@@ -69375,17 +69456,17 @@
       <c r="AD277" t="s">
         <v>40</v>
       </c>
-      <c r="AE277" t="s">
-        <v>40</v>
+      <c r="AE277" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF277" t="s">
         <v>40</v>
       </c>
-      <c r="AG277" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH277" t="s">
-        <v>40</v>
+      <c r="AG277" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH277" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI277" t="s">
         <v>40</v>
@@ -69418,7 +69499,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="278" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="278" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A278" t="s">
         <v>2581</v>
       </c>
@@ -69509,17 +69590,17 @@
       <c r="AD278" t="s">
         <v>40</v>
       </c>
-      <c r="AE278" t="s">
-        <v>40</v>
+      <c r="AE278" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF278" t="s">
         <v>40</v>
       </c>
-      <c r="AG278" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH278" t="s">
-        <v>40</v>
+      <c r="AG278" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH278" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI278" t="s">
         <v>40</v>
@@ -69552,7 +69633,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="279" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="279" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A279" t="s">
         <v>2581</v>
       </c>
@@ -69643,17 +69724,17 @@
       <c r="AD279" t="s">
         <v>40</v>
       </c>
-      <c r="AE279" t="s">
-        <v>40</v>
+      <c r="AE279" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF279" t="s">
         <v>40</v>
       </c>
-      <c r="AG279" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH279" t="s">
-        <v>40</v>
+      <c r="AG279" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH279" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI279" t="s">
         <v>40</v>
@@ -69686,7 +69767,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="280" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="280" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A280" t="s">
         <v>2581</v>
       </c>
@@ -69774,20 +69855,20 @@
       <c r="AC280">
         <v>14</v>
       </c>
-      <c r="AD280" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE280" t="s">
-        <v>40</v>
+      <c r="AD280" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE280" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF280" t="s">
         <v>40</v>
       </c>
-      <c r="AG280" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH280" t="s">
-        <v>40</v>
+      <c r="AG280" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH280" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI280" t="s">
         <v>40</v>
@@ -69820,7 +69901,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="281" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="281" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A281" t="s">
         <v>2581</v>
       </c>
@@ -69908,20 +69989,20 @@
       <c r="AC281">
         <v>14</v>
       </c>
-      <c r="AD281" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE281" t="s">
-        <v>40</v>
+      <c r="AD281" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE281" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF281" t="s">
         <v>40</v>
       </c>
-      <c r="AG281" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH281" t="s">
-        <v>40</v>
+      <c r="AG281" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH281" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI281" t="s">
         <v>40</v>
@@ -69954,7 +70035,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="282" spans="1:44" x14ac:dyDescent="0.5">
+    <row r="282" spans="1:45" x14ac:dyDescent="0.5">
       <c r="A282" t="s">
         <v>2581</v>
       </c>
@@ -70042,20 +70123,20 @@
       <c r="AC282">
         <v>14</v>
       </c>
-      <c r="AD282" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE282" t="s">
-        <v>40</v>
+      <c r="AD282" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE282" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AF282" t="s">
         <v>40</v>
       </c>
-      <c r="AG282" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH282" t="s">
-        <v>40</v>
+      <c r="AG282" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH282" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="AI282" t="s">
         <v>40</v>
@@ -70086,6 +70167,1887 @@
       </c>
       <c r="AR282" t="s">
         <v>2644</v>
+      </c>
+    </row>
+    <row r="283" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A283" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B283" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C283" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D283" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E283" t="s">
+        <v>673</v>
+      </c>
+      <c r="F283" t="s">
+        <v>39</v>
+      </c>
+      <c r="G283" t="s">
+        <v>41</v>
+      </c>
+      <c r="H283" t="s">
+        <v>40</v>
+      </c>
+      <c r="I283" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J283" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K283" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L283">
+        <v>173</v>
+      </c>
+      <c r="M283" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N283" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O283">
+        <v>2012</v>
+      </c>
+      <c r="P283">
+        <v>2013</v>
+      </c>
+      <c r="Q283" t="s">
+        <v>2710</v>
+      </c>
+      <c r="R283">
+        <v>0</v>
+      </c>
+      <c r="S283" t="s">
+        <v>39</v>
+      </c>
+      <c r="T283" t="s">
+        <v>39</v>
+      </c>
+      <c r="U283" t="s">
+        <v>2630</v>
+      </c>
+      <c r="V283" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="W283" t="s">
+        <v>39</v>
+      </c>
+      <c r="X283" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y283" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z283" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA283" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB283" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC283" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD283" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE283" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF283" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG283" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH283" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI283" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ283" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK283">
+        <v>26.37</v>
+      </c>
+      <c r="AL283" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM283">
+        <v>3.67</v>
+      </c>
+      <c r="AN283">
+        <v>4</v>
+      </c>
+      <c r="AO283">
+        <v>500</v>
+      </c>
+      <c r="AP283">
+        <v>30</v>
+      </c>
+      <c r="AQ283" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR283" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="284" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A284" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B284" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C284" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D284" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E284" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G284" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H284" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I284" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J284" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K284" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L284" s="15">
+        <v>173</v>
+      </c>
+      <c r="M284" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O284" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P284" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q284" s="15" t="s">
+        <v>2696</v>
+      </c>
+      <c r="R284" s="15">
+        <v>30</v>
+      </c>
+      <c r="S284" s="15" t="s">
+        <v>2697</v>
+      </c>
+      <c r="T284" s="15">
+        <v>4</v>
+      </c>
+      <c r="U284" s="15" t="s">
+        <v>2703</v>
+      </c>
+      <c r="V284" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X284" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z284" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD284" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF284" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH284" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI284" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ284" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK284" s="15">
+        <v>58.68</v>
+      </c>
+      <c r="AL284" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM284" s="15">
+        <v>7.78</v>
+      </c>
+      <c r="AN284" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO284" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP284" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ284" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR284" s="15" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="285" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A285" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B285" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C285" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D285" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E285" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G285" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H285" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I285" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J285" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K285" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L285" s="15">
+        <v>173</v>
+      </c>
+      <c r="M285" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O285" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P285" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q285" s="15" t="s">
+        <v>2698</v>
+      </c>
+      <c r="R285" s="15">
+        <v>30</v>
+      </c>
+      <c r="S285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="T285" s="15">
+        <v>4</v>
+      </c>
+      <c r="U285" s="15" t="s">
+        <v>2704</v>
+      </c>
+      <c r="V285" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X285" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z285" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD285" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF285" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH285" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI285" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ285" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK285" s="15">
+        <v>54.44</v>
+      </c>
+      <c r="AL285" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM285" s="15">
+        <v>3.33</v>
+      </c>
+      <c r="AN285" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO285" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP285" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ285" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR285" s="15" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="286" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A286" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B286" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C286" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D286" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E286" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G286" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H286" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I286" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J286" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K286" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L286" s="15">
+        <v>173</v>
+      </c>
+      <c r="M286" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O286" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P286" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q286" s="15" t="s">
+        <v>2699</v>
+      </c>
+      <c r="R286" s="15">
+        <v>30</v>
+      </c>
+      <c r="S286" s="15">
+        <v>75</v>
+      </c>
+      <c r="T286" s="15" t="s">
+        <v>2700</v>
+      </c>
+      <c r="U286" s="15" t="s">
+        <v>2705</v>
+      </c>
+      <c r="V286" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X286" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z286" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD286" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF286" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH286" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI286" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ286" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK286" s="15">
+        <v>22.36</v>
+      </c>
+      <c r="AL286" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM286" s="15">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AN286" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO286" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP286" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ286" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR286" s="15" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="287" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A287" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B287" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C287" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D287" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E287" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G287" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H287" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I287" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J287" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K287" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L287" s="15">
+        <v>173</v>
+      </c>
+      <c r="M287" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O287" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P287" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q287" s="15" t="s">
+        <v>2701</v>
+      </c>
+      <c r="R287" s="15">
+        <v>30</v>
+      </c>
+      <c r="S287" s="15">
+        <v>75</v>
+      </c>
+      <c r="T287" s="15" t="s">
+        <v>2702</v>
+      </c>
+      <c r="U287" s="15" t="s">
+        <v>2706</v>
+      </c>
+      <c r="V287" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X287" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z287" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD287" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF287" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH287" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI287" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ287" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK287" s="15">
+        <v>25.76</v>
+      </c>
+      <c r="AL287" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM287" s="15">
+        <v>8.68</v>
+      </c>
+      <c r="AN287" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO287" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP287" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ287" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR287" s="15" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="288" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A288" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B288" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C288" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D288" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E288" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G288" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H288" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I288" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J288" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K288" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L288" s="15">
+        <v>173</v>
+      </c>
+      <c r="M288" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O288" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P288" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q288" s="15" t="s">
+        <v>2707</v>
+      </c>
+      <c r="R288" s="15">
+        <v>30</v>
+      </c>
+      <c r="S288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="T288" s="15">
+        <v>5</v>
+      </c>
+      <c r="U288" s="15" t="s">
+        <v>2612</v>
+      </c>
+      <c r="V288" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X288" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z288" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD288" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF288" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH288" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI288" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ288" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK288" s="15">
+        <v>89.32</v>
+      </c>
+      <c r="AL288" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM288" s="15">
+        <v>3.33</v>
+      </c>
+      <c r="AN288" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO288" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP288" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ288" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR288" s="15" t="s">
+        <v>2617</v>
+      </c>
+      <c r="AS288" s="15"/>
+    </row>
+    <row r="289" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A289" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B289" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C289" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D289" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E289" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G289" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H289" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I289" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J289" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K289" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L289" s="15">
+        <v>173</v>
+      </c>
+      <c r="M289" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O289" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P289" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q289" s="15" t="s">
+        <v>2696</v>
+      </c>
+      <c r="R289" s="15">
+        <v>60</v>
+      </c>
+      <c r="S289" s="15" t="s">
+        <v>2697</v>
+      </c>
+      <c r="T289" s="15">
+        <v>4</v>
+      </c>
+      <c r="U289" s="15" t="s">
+        <v>2703</v>
+      </c>
+      <c r="V289" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X289" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z289" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD289" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF289" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH289" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI289" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ289" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK289" s="15">
+        <v>57.78</v>
+      </c>
+      <c r="AL289" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM289" s="15">
+        <v>4.01</v>
+      </c>
+      <c r="AN289" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO289" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP289" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ289" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR289" s="15" t="s">
+        <v>2617</v>
+      </c>
+      <c r="AS289" s="15"/>
+    </row>
+    <row r="290" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A290" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B290" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C290" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D290" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E290" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G290" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H290" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I290" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J290" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K290" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L290" s="15">
+        <v>173</v>
+      </c>
+      <c r="M290" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O290" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P290" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q290" s="15" t="s">
+        <v>2698</v>
+      </c>
+      <c r="R290" s="15">
+        <v>60</v>
+      </c>
+      <c r="S290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="T290" s="15">
+        <v>4</v>
+      </c>
+      <c r="U290" s="15" t="s">
+        <v>2704</v>
+      </c>
+      <c r="V290" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X290" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z290" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD290" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF290" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH290" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI290" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ290" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK290" s="15">
+        <v>54.45</v>
+      </c>
+      <c r="AL290" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM290" s="15">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AN290" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO290" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP290" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ290" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR290" s="15" t="s">
+        <v>2617</v>
+      </c>
+      <c r="AS290" s="15"/>
+    </row>
+    <row r="291" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A291" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B291" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C291" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D291" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E291" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G291" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H291" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I291" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J291" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K291" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L291" s="15">
+        <v>173</v>
+      </c>
+      <c r="M291" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O291" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P291" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q291" s="15" t="s">
+        <v>2699</v>
+      </c>
+      <c r="R291" s="15">
+        <v>60</v>
+      </c>
+      <c r="S291" s="15">
+        <v>75</v>
+      </c>
+      <c r="T291" s="15" t="s">
+        <v>2700</v>
+      </c>
+      <c r="U291" s="15" t="s">
+        <v>2705</v>
+      </c>
+      <c r="V291" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X291" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z291" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD291" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF291" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH291" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI291" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ291" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK291" s="15">
+        <v>43.76</v>
+      </c>
+      <c r="AL291" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM291" s="15">
+        <v>2.16</v>
+      </c>
+      <c r="AN291" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO291" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP291" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ291" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR291" s="15" t="s">
+        <v>2617</v>
+      </c>
+      <c r="AS291" s="15"/>
+    </row>
+    <row r="292" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A292" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B292" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C292" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D292" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E292" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G292" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H292" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I292" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J292" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K292" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L292" s="15">
+        <v>173</v>
+      </c>
+      <c r="M292" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O292" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P292" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q292" s="15" t="s">
+        <v>2701</v>
+      </c>
+      <c r="R292" s="15">
+        <v>60</v>
+      </c>
+      <c r="S292" s="15">
+        <v>75</v>
+      </c>
+      <c r="T292" s="15" t="s">
+        <v>2702</v>
+      </c>
+      <c r="U292" s="15" t="s">
+        <v>2706</v>
+      </c>
+      <c r="V292" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X292" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z292" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD292" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF292" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH292" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI292" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ292" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK292" s="15">
+        <v>41.44</v>
+      </c>
+      <c r="AL292" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM292" s="15">
+        <v>1.25</v>
+      </c>
+      <c r="AN292" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO292" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP292" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ292" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR292" s="15" t="s">
+        <v>2617</v>
+      </c>
+      <c r="AS292" s="15"/>
+    </row>
+    <row r="293" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A293" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B293" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C293" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D293" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E293" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G293" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H293" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I293" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J293" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K293" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L293" s="15">
+        <v>173</v>
+      </c>
+      <c r="M293" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O293" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P293" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q293" s="15" t="s">
+        <v>2696</v>
+      </c>
+      <c r="R293" s="15">
+        <v>90</v>
+      </c>
+      <c r="S293" s="15" t="s">
+        <v>2697</v>
+      </c>
+      <c r="T293" s="15">
+        <v>4</v>
+      </c>
+      <c r="U293" s="15" t="s">
+        <v>2703</v>
+      </c>
+      <c r="V293" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X293" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z293" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD293" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF293" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH293" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI293" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ293" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK293" s="15">
+        <v>63.33</v>
+      </c>
+      <c r="AL293" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM293" s="15">
+        <v>6.94</v>
+      </c>
+      <c r="AN293" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO293" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP293" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ293" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR293" s="15" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="294" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A294" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B294" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C294" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D294" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E294" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G294" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H294" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I294" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J294" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K294" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L294" s="15">
+        <v>173</v>
+      </c>
+      <c r="M294" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O294" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P294" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q294" s="15" t="s">
+        <v>2698</v>
+      </c>
+      <c r="R294" s="15">
+        <v>90</v>
+      </c>
+      <c r="S294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="T294" s="15">
+        <v>4</v>
+      </c>
+      <c r="U294" s="15" t="s">
+        <v>2704</v>
+      </c>
+      <c r="V294" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X294" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z294" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD294" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF294" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH294" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI294" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ294" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK294" s="15">
+        <v>70.650000000000006</v>
+      </c>
+      <c r="AL294" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM294" s="15">
+        <v>2.63</v>
+      </c>
+      <c r="AN294" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO294" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP294" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ294" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR294" s="15" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="295" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A295" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B295" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C295" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D295" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E295" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G295" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H295" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I295" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J295" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K295" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L295" s="15">
+        <v>173</v>
+      </c>
+      <c r="M295" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O295" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P295" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q295" s="15" t="s">
+        <v>2699</v>
+      </c>
+      <c r="R295" s="15">
+        <v>90</v>
+      </c>
+      <c r="S295" s="15">
+        <v>75</v>
+      </c>
+      <c r="T295" s="15" t="s">
+        <v>2700</v>
+      </c>
+      <c r="U295" s="15" t="s">
+        <v>2705</v>
+      </c>
+      <c r="V295" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X295" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z295" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD295" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF295" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI295" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ295" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK295" s="15">
+        <v>42.65</v>
+      </c>
+      <c r="AL295" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM295" s="15">
+        <v>3.33</v>
+      </c>
+      <c r="AN295" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO295" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP295" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ295" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR295" s="15" t="s">
+        <v>2617</v>
+      </c>
+    </row>
+    <row r="296" spans="1:45" x14ac:dyDescent="0.5">
+      <c r="A296" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B296" s="15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C296" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="D296" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E296" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="F296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G296" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H296" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I296" s="15" t="s">
+        <v>2694</v>
+      </c>
+      <c r="J296" s="15" t="s">
+        <v>2693</v>
+      </c>
+      <c r="K296" s="15" t="s">
+        <v>2692</v>
+      </c>
+      <c r="L296" s="15">
+        <v>173</v>
+      </c>
+      <c r="M296" s="15" t="s">
+        <v>2597</v>
+      </c>
+      <c r="N296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O296" s="15">
+        <v>2012</v>
+      </c>
+      <c r="P296" s="15">
+        <v>2013</v>
+      </c>
+      <c r="Q296" s="15" t="s">
+        <v>2701</v>
+      </c>
+      <c r="R296" s="15">
+        <v>90</v>
+      </c>
+      <c r="S296" s="15">
+        <v>75</v>
+      </c>
+      <c r="T296" s="15" t="s">
+        <v>2702</v>
+      </c>
+      <c r="U296" s="15" t="s">
+        <v>2706</v>
+      </c>
+      <c r="V296" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="W296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X296" s="15" t="s">
+        <v>2708</v>
+      </c>
+      <c r="Y296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z296" s="15" t="s">
+        <v>2709</v>
+      </c>
+      <c r="AA296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD296" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF296" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH296" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI296" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ296" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK296" s="15">
+        <v>51.11</v>
+      </c>
+      <c r="AL296" s="15" t="s">
+        <v>2695</v>
+      </c>
+      <c r="AM296" s="15">
+        <v>2.94</v>
+      </c>
+      <c r="AN296" s="15">
+        <v>4</v>
+      </c>
+      <c r="AO296" s="15">
+        <v>500</v>
+      </c>
+      <c r="AP296" s="15">
+        <v>30</v>
+      </c>
+      <c r="AQ296" s="15" t="s">
+        <v>2605</v>
+      </c>
+      <c r="AR296" s="15" t="s">
+        <v>2617</v>
       </c>
     </row>
   </sheetData>
@@ -70098,10 +72060,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:U86"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="72" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64:G68"/>
+    <sheetView topLeftCell="A40" zoomScale="72" workbookViewId="0">
+      <selection activeCell="S73" sqref="S73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -71226,7 +73188,7 @@
         <v>93.617999999999995</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>2</v>
       </c>
@@ -71249,7 +73211,7 @@
         <v>94.584000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>3</v>
       </c>
@@ -71272,7 +73234,7 @@
         <v>94.584000000000003</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>4</v>
       </c>
@@ -71295,7 +73257,7 @@
         <v>98.539000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>5</v>
       </c>
@@ -71318,8 +73280,826 @@
         <v>97.100999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="F80" s="1"/>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A72" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E72" s="14">
+        <v>24</v>
+      </c>
+      <c r="F72" s="14">
+        <v>1</v>
+      </c>
+      <c r="G72" s="14">
+        <v>59</v>
+      </c>
+      <c r="H72" s="14">
+        <v>2007</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>1201</v>
+      </c>
+      <c r="J72" s="14" t="s">
+        <v>1202</v>
+      </c>
+      <c r="K72" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="14"/>
+      <c r="P72" s="14" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q72" s="14"/>
+      <c r="R72" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="S72" s="14" t="s">
+        <v>1203</v>
+      </c>
+      <c r="T72" s="14" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U72" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A73" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E73" s="15">
+        <v>37</v>
+      </c>
+      <c r="F73" s="15">
+        <v>10</v>
+      </c>
+      <c r="G73" s="15">
+        <v>2033</v>
+      </c>
+      <c r="H73" s="15">
+        <v>2017</v>
+      </c>
+      <c r="I73" s="15" t="s">
+        <v>1207</v>
+      </c>
+      <c r="J73" s="15" t="s">
+        <v>673</v>
+      </c>
+      <c r="K73" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S73" s="15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="T73" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U73" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A74" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>825</v>
+      </c>
+      <c r="E74" s="15">
+        <v>38</v>
+      </c>
+      <c r="F74" s="15">
+        <v>2</v>
+      </c>
+      <c r="G74" s="15">
+        <v>57</v>
+      </c>
+      <c r="H74" s="15">
+        <v>2014</v>
+      </c>
+      <c r="I74" s="15" t="s">
+        <v>1211</v>
+      </c>
+      <c r="J74" s="15" t="s">
+        <v>1212</v>
+      </c>
+      <c r="K74" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S74" s="15" t="s">
+        <v>1213</v>
+      </c>
+      <c r="T74" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U74" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A75" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E75" s="15">
+        <v>13</v>
+      </c>
+      <c r="F75" s="15">
+        <v>6</v>
+      </c>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15">
+        <v>2021</v>
+      </c>
+      <c r="I75" s="15" t="s">
+        <v>1217</v>
+      </c>
+      <c r="J75" s="15" t="s">
+        <v>1218</v>
+      </c>
+      <c r="K75" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S75" s="15" t="s">
+        <v>1219</v>
+      </c>
+      <c r="T75" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U75" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A76" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="E76" s="15">
+        <v>291</v>
+      </c>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15">
+        <v>2022</v>
+      </c>
+      <c r="I76" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="J76" s="15" t="s">
+        <v>1222</v>
+      </c>
+      <c r="K76" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S76" s="15" t="s">
+        <v>1223</v>
+      </c>
+      <c r="T76" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U76" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A77" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E77" s="15">
+        <v>39</v>
+      </c>
+      <c r="F77" s="15">
+        <v>1</v>
+      </c>
+      <c r="G77" s="15">
+        <v>82</v>
+      </c>
+      <c r="H77" s="15">
+        <v>2011</v>
+      </c>
+      <c r="I77" s="15" t="s">
+        <v>1226</v>
+      </c>
+      <c r="J77" s="15" t="s">
+        <v>1227</v>
+      </c>
+      <c r="K77" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S77" s="15" t="s">
+        <v>1197</v>
+      </c>
+      <c r="T77" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U77" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A78" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>1230</v>
+      </c>
+      <c r="E78" s="15">
+        <v>44</v>
+      </c>
+      <c r="F78" s="15">
+        <v>6</v>
+      </c>
+      <c r="G78" s="15">
+        <v>14</v>
+      </c>
+      <c r="H78" s="15">
+        <v>2016</v>
+      </c>
+      <c r="I78" s="15" t="s">
+        <v>1231</v>
+      </c>
+      <c r="J78" s="15" t="s">
+        <v>1232</v>
+      </c>
+      <c r="K78" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S78" s="15" t="s">
+        <v>1233</v>
+      </c>
+      <c r="T78" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U78" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A79" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E79" s="15">
+        <v>15</v>
+      </c>
+      <c r="F79" s="15">
+        <v>1</v>
+      </c>
+      <c r="G79" s="15">
+        <v>39</v>
+      </c>
+      <c r="H79" s="15">
+        <v>2010</v>
+      </c>
+      <c r="I79" s="15" t="s">
+        <v>1237</v>
+      </c>
+      <c r="J79" s="15" t="s">
+        <v>1238</v>
+      </c>
+      <c r="K79" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
+      <c r="P79" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q79" s="15"/>
+      <c r="R79" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S79" s="15" t="s">
+        <v>1239</v>
+      </c>
+      <c r="T79" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U79" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A80" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="E80" s="15">
+        <v>28</v>
+      </c>
+      <c r="F80" s="15">
+        <v>2</v>
+      </c>
+      <c r="G80" s="15">
+        <v>253</v>
+      </c>
+      <c r="H80" s="15">
+        <v>2015</v>
+      </c>
+      <c r="I80" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="J80" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="K80" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15"/>
+      <c r="P80" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q80" s="15"/>
+      <c r="R80" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S80" s="15" t="s">
+        <v>1242</v>
+      </c>
+      <c r="T80" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U80" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A81" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="E81" s="15">
+        <v>11</v>
+      </c>
+      <c r="F81" s="15">
+        <v>4</v>
+      </c>
+      <c r="G81" s="15">
+        <v>373</v>
+      </c>
+      <c r="H81" s="15">
+        <v>1996</v>
+      </c>
+      <c r="I81" s="15" t="s">
+        <v>1250</v>
+      </c>
+      <c r="J81" s="15" t="s">
+        <v>1251</v>
+      </c>
+      <c r="K81" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15"/>
+      <c r="P81" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q81" s="15"/>
+      <c r="R81" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S81" s="15" t="s">
+        <v>1252</v>
+      </c>
+      <c r="T81" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U81" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A82" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>1255</v>
+      </c>
+      <c r="E82" s="15">
+        <v>8</v>
+      </c>
+      <c r="F82" s="15">
+        <v>2</v>
+      </c>
+      <c r="G82" s="15">
+        <v>143</v>
+      </c>
+      <c r="H82" s="15">
+        <v>1993</v>
+      </c>
+      <c r="I82" s="15" t="s">
+        <v>1256</v>
+      </c>
+      <c r="J82" s="15" t="s">
+        <v>1257</v>
+      </c>
+      <c r="K82" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="O82" s="15"/>
+      <c r="P82" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q82" s="15"/>
+      <c r="R82" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S82" s="15" t="s">
+        <v>1258</v>
+      </c>
+      <c r="T82" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U82" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A83" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>947</v>
+      </c>
+      <c r="E83" s="15">
+        <v>36</v>
+      </c>
+      <c r="F83" s="15">
+        <v>4</v>
+      </c>
+      <c r="G83" s="15">
+        <v>15</v>
+      </c>
+      <c r="H83" s="15">
+        <v>2016</v>
+      </c>
+      <c r="I83" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="J83" s="15" t="s">
+        <v>860</v>
+      </c>
+      <c r="K83" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L83" s="15"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="O83" s="15"/>
+      <c r="P83" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q83" s="15"/>
+      <c r="R83" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S83" s="15" t="s">
+        <v>1261</v>
+      </c>
+      <c r="T83" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U83" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A84" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E84" s="15">
+        <v>32</v>
+      </c>
+      <c r="F84" s="15">
+        <v>1</v>
+      </c>
+      <c r="G84" s="15">
+        <v>69</v>
+      </c>
+      <c r="H84" s="15">
+        <v>2012</v>
+      </c>
+      <c r="I84" s="15" t="s">
+        <v>1265</v>
+      </c>
+      <c r="J84" s="15" t="s">
+        <v>1266</v>
+      </c>
+      <c r="K84" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L84" s="15"/>
+      <c r="M84" s="15"/>
+      <c r="N84" s="15"/>
+      <c r="O84" s="15"/>
+      <c r="P84" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q84" s="15"/>
+      <c r="R84" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S84" s="15" t="s">
+        <v>1267</v>
+      </c>
+      <c r="T84" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U84" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A85" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="E85" s="15">
+        <v>13</v>
+      </c>
+      <c r="F85" s="15">
+        <v>4</v>
+      </c>
+      <c r="G85" s="15">
+        <v>55</v>
+      </c>
+      <c r="H85" s="15">
+        <v>2004</v>
+      </c>
+      <c r="I85" s="15" t="s">
+        <v>1270</v>
+      </c>
+      <c r="J85" s="15" t="s">
+        <v>1271</v>
+      </c>
+      <c r="K85" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="L85" s="15"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q85" s="15"/>
+      <c r="R85" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="S85" s="15" t="s">
+        <v>1272</v>
+      </c>
+      <c r="T85" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U85" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.5">
+      <c r="A86" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>962</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>963</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E86" s="15">
+        <v>42</v>
+      </c>
+      <c r="F86" s="15">
+        <v>3</v>
+      </c>
+      <c r="G86" s="15">
+        <v>466</v>
+      </c>
+      <c r="H86" s="15">
+        <v>2014</v>
+      </c>
+      <c r="I86" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="J86" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="K86" s="15" t="s">
+        <v>964</v>
+      </c>
+      <c r="L86" s="15"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="15"/>
+      <c r="O86" s="15"/>
+      <c r="P86" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q86" s="15" t="s">
+        <v>965</v>
+      </c>
+      <c r="R86" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="S86" s="15" t="s">
+        <v>966</v>
+      </c>
+      <c r="T86" s="15" t="s">
+        <v>2595</v>
+      </c>
+      <c r="U86" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>